<commit_message>
[Pipette] Issue note format 수정
</commit_message>
<xml_diff>
--- a/Plasma_Gen_Issue Note.xlsx
+++ b/Plasma_Gen_Issue Note.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="122211" calcMode="manual"/>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
@@ -358,7 +358,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -434,6 +434,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -739,10 +742,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H32"/>
+  <dimension ref="B1:H31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -759,104 +762,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="26" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="9" t="s">
+    <row r="2" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H3" s="10" t="s">
         <v>4</v>
       </c>
     </row>
+    <row r="4" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="11">
+        <v>43153</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
     <row r="5" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B5" s="2">
-        <v>1</v>
-      </c>
-      <c r="C5" s="11">
-        <v>43153</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="B5" s="4">
+        <v>2</v>
+      </c>
+      <c r="C5" s="14">
+        <v>43154</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="F5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" s="14">
         <v>43154</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="21" t="s">
-        <v>13</v>
-      </c>
+      <c r="G6" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="16"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
-        <v>3</v>
-      </c>
-      <c r="C7" s="14">
-        <v>43154</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>17</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="15"/>
       <c r="H7" s="16"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="5"/>
@@ -867,7 +881,7 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="5"/>
@@ -878,7 +892,7 @@
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="5"/>
@@ -889,7 +903,7 @@
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="5"/>
@@ -900,7 +914,7 @@
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="5"/>
@@ -911,7 +925,7 @@
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="5"/>
@@ -922,7 +936,7 @@
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="5"/>
@@ -933,7 +947,7 @@
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="5"/>
@@ -944,7 +958,7 @@
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="5"/>
@@ -955,7 +969,7 @@
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="4">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C17" s="14"/>
       <c r="D17" s="5"/>
@@ -966,7 +980,7 @@
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" s="4">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C18" s="14"/>
       <c r="D18" s="5"/>
@@ -977,7 +991,7 @@
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C19" s="14"/>
       <c r="D19" s="5"/>
@@ -988,7 +1002,7 @@
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="4">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C20" s="14"/>
       <c r="D20" s="5"/>
@@ -999,7 +1013,7 @@
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="4">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C21" s="14"/>
       <c r="D21" s="5"/>
@@ -1010,7 +1024,7 @@
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C22" s="14"/>
       <c r="D22" s="5"/>
@@ -1021,7 +1035,7 @@
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23" s="4">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C23" s="14"/>
       <c r="D23" s="5"/>
@@ -1032,7 +1046,7 @@
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B24" s="4">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C24" s="14"/>
       <c r="D24" s="5"/>
@@ -1043,7 +1057,7 @@
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B25" s="4">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C25" s="14"/>
       <c r="D25" s="5"/>
@@ -1054,7 +1068,7 @@
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B26" s="4">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C26" s="14"/>
       <c r="D26" s="5"/>
@@ -1065,7 +1079,7 @@
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B27" s="4">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C27" s="14"/>
       <c r="D27" s="5"/>
@@ -1076,7 +1090,7 @@
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B28" s="4">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C28" s="14"/>
       <c r="D28" s="5"/>
@@ -1087,7 +1101,7 @@
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B29" s="4">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C29" s="14"/>
       <c r="D29" s="5"/>
@@ -1098,7 +1112,7 @@
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B30" s="4">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C30" s="14"/>
       <c r="D30" s="5"/>
@@ -1107,41 +1121,30 @@
       <c r="G30" s="15"/>
       <c r="H30" s="16"/>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B31" s="4">
-        <v>27</v>
-      </c>
-      <c r="C31" s="14"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="16"/>
-    </row>
-    <row r="32" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="6">
+    <row r="31" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="6">
         <v>28</v>
       </c>
-      <c r="C32" s="17"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="19"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="19"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="65" orientation="landscape" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H32"/>
+  <dimension ref="B1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1152,66 +1155,77 @@
     <col min="4" max="4" width="12.625" style="22" customWidth="1"/>
     <col min="5" max="5" width="9.75" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.875" style="8" customWidth="1"/>
-    <col min="7" max="7" width="47.875" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="46.375" style="8" customWidth="1"/>
     <col min="8" max="8" width="59" style="8" customWidth="1"/>
     <col min="9" max="16384" width="9" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="26" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="9" t="s">
+    <row r="2" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H3" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B5" s="2">
+    <row r="4" spans="2:8" ht="33" x14ac:dyDescent="0.3">
+      <c r="B4" s="2">
         <v>1</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C4" s="11">
         <v>43153</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D4" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H4" s="13" t="s">
         <v>8</v>
       </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="4">
+        <v>2</v>
+      </c>
+      <c r="C5" s="14"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="16"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="24"/>
@@ -1222,7 +1236,7 @@
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="24"/>
@@ -1233,7 +1247,7 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="24"/>
@@ -1244,7 +1258,7 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="24"/>
@@ -1255,7 +1269,7 @@
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="24"/>
@@ -1266,7 +1280,7 @@
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="24"/>
@@ -1277,7 +1291,7 @@
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="24"/>
@@ -1288,7 +1302,7 @@
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="24"/>
@@ -1299,7 +1313,7 @@
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="24"/>
@@ -1310,7 +1324,7 @@
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="24"/>
@@ -1321,7 +1335,7 @@
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="24"/>
@@ -1332,7 +1346,7 @@
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="4">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C17" s="14"/>
       <c r="D17" s="24"/>
@@ -1343,7 +1357,7 @@
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" s="4">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C18" s="14"/>
       <c r="D18" s="24"/>
@@ -1354,7 +1368,7 @@
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C19" s="14"/>
       <c r="D19" s="24"/>
@@ -1365,7 +1379,7 @@
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="4">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C20" s="14"/>
       <c r="D20" s="24"/>
@@ -1376,7 +1390,7 @@
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="4">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C21" s="14"/>
       <c r="D21" s="24"/>
@@ -1387,7 +1401,7 @@
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C22" s="14"/>
       <c r="D22" s="24"/>
@@ -1398,7 +1412,7 @@
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23" s="4">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C23" s="14"/>
       <c r="D23" s="24"/>
@@ -1409,7 +1423,7 @@
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B24" s="4">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C24" s="14"/>
       <c r="D24" s="24"/>
@@ -1420,7 +1434,7 @@
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B25" s="4">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C25" s="14"/>
       <c r="D25" s="24"/>
@@ -1431,7 +1445,7 @@
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B26" s="4">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C26" s="14"/>
       <c r="D26" s="24"/>
@@ -1442,7 +1456,7 @@
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B27" s="4">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C27" s="14"/>
       <c r="D27" s="24"/>
@@ -1453,7 +1467,7 @@
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B28" s="4">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C28" s="14"/>
       <c r="D28" s="24"/>
@@ -1464,7 +1478,7 @@
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B29" s="4">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C29" s="14"/>
       <c r="D29" s="24"/>
@@ -1475,7 +1489,7 @@
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B30" s="4">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C30" s="14"/>
       <c r="D30" s="24"/>
@@ -1484,32 +1498,21 @@
       <c r="G30" s="15"/>
       <c r="H30" s="16"/>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B31" s="4">
-        <v>27</v>
-      </c>
-      <c r="C31" s="14"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="16"/>
-    </row>
-    <row r="32" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="6">
+    <row r="31" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="6">
         <v>28</v>
       </c>
-      <c r="C32" s="17"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="19"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="19"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="73" orientation="landscape" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
[DOC]Issue update - Transformer
</commit_message>
<xml_diff>
--- a/Plasma_Gen_Issue Note.xlsx
+++ b/Plasma_Gen_Issue Note.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
   <si>
     <t>No</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -119,7 +119,41 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>외부 GND 연결용 Jack 추가 - ear jack type</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>V1.0 -A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>V1.0 -B,C</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Open</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma 발생 안함
+Gas 주입 상태에서도 발생 안함</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>전압을 올려보며 시험 필요</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SCH</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTX2106xx series의 2차측 구조가 datasheet와 틀림
+- 2차측이 2개로 나눠져 있는것으로 보임</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>V1.0</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -498,7 +532,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -533,7 +567,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -745,7 +779,7 @@
   <dimension ref="B1:H31"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -861,11 +895,21 @@
       <c r="B7" s="4">
         <v>4</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="15"/>
+      <c r="C7" s="14">
+        <v>43158</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>23</v>
+      </c>
       <c r="H7" s="16"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
@@ -1144,7 +1188,7 @@
   <dimension ref="B1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1197,7 +1241,7 @@
         <v>43153</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>5</v>
@@ -1212,27 +1256,49 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" ht="33" x14ac:dyDescent="0.3">
       <c r="B5" s="4">
         <v>2</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="15"/>
+      <c r="C5" s="14">
+        <v>43153</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>30</v>
+      </c>
       <c r="H5" s="16"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" ht="33" x14ac:dyDescent="0.3">
       <c r="B6" s="4">
         <v>3</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="16"/>
+      <c r="C6" s="14">
+        <v>43158</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="4">

</xml_diff>

<commit_message>
[DOC] Femto 진행 item 추가
</commit_message>
<xml_diff>
--- a/Plasma_Gen_Issue Note.xlsx
+++ b/Plasma_Gen_Issue Note.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Check list" sheetId="2" r:id="rId1"/>
@@ -168,10 +168,6 @@
   <si>
     <t>S/V sample이 항상 through 되어 있음
  - 형상 검토용 sample로 보임 : Femto 확인 필요</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reset IC 추가 - Voltage drop에 의한 MCU halt 방지</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -294,6 +290,136 @@
   </si>
   <si>
     <t>Booster over voltage protect 기능 확인</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Transformer에서 Timer path로 Over voltage 또는 Over Current 발생할 수 있음 - Protection circuit 추가 필요
+ - Timer path에 Series Resistor 추가 필요
+ - Zener diode 추가 - 5V 
+    : BZT52C5V1S or CZRQR52C5V1-HF</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>교수님 장비 사용</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oscilloscope, Probe 2ea, Power supply 1ea</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>멀티미터 1ea</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Femto에서 제공</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Computer 1ea , LCD 2ea</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>모델 선정 후 통보</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma 장비 - LF 1ea, RF 1ea, Pipette Test용 Gas</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>대여</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>부동산 계약</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>인터넷 신청, 아파트 관리사무소 신고, 도시가스 신청</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>개인적으로 신청후 영수증 제출</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>부자제</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pipette D/L용 USB cable 구매</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Main PCB - Top 방향으로 배치 ( 3/29 Femto 협의)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DC Jack 인식을 위한 interface 추가</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Key 추가, Pin 1ea 추가</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pipette</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>V1.0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>OPEN</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>S/V 구매 - Series LX-Value_8mm</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Target</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>S/V 부자재 구매 - Gasket, 12'' Wire lead, Screw</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fitting 선정 및 구매</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Needle 선정 및 구매</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>S/V 기능 확인을 위한 Sample 요청 - Femto
+ - 구매 진행중</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>needle 선정 및 구매</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>기구물</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>악어클립은 사용하지 않음
+전용 GND 판 제작 예정</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GND 판과의 연결 방법 협의 - 일단 악어클립으로 제작
+  - 악어클립 or Ring 단자</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GND 판과의 연결 방법 협의</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -317,138 +443,12 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Transformer에서 Timer path로 Over voltage 또는 Over Current 발생할 수 있음 - Protection circuit 추가 필요
- - Timer path에 Series Resistor 추가 필요
- - Zener diode 추가 - 5V 
-    : BZT52C5V1S or CZRQR52C5V1-HF</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Timer path에 Series Resistor, Zener diode(BZT52C5V1S) 추가
 S/V 전원에 Zener diode(BZT52C5V1S) 추가</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>교수님 장비 사용</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Oscilloscope, Probe 2ea, Power supply 1ea</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>멀티미터 1ea</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Femto에서 제공</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Computer 1ea , LCD 2ea</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>모델 선정 후 통보</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Plasma 장비 - LF 1ea, RF 1ea, Pipette Test용 Gas</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>대여</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>부동산 계약</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>인터넷 신청, 아파트 관리사무소 신고, 도시가스 신청</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>개인적으로 신청후 영수증 제출</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>부자제</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pipette D/L용 USB cable 구매</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Main PCB - Top 방향으로 배치 ( 3/29 Femto 협의)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>DC Jack 인식을 위한 interface 추가</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Key 추가, Pin 1ea 추가</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pipette</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>V1.0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>OPEN</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>S/V 구매 - Series LX-Value_8mm</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Target</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>S/V 부자재 구매 - Gasket, 12'' Wire lead, Screw</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fitting 선정 및 구매</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Needle 선정 및 구매</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>S/V 기능 확인을 위한 Sample 요청 - Femto
- - 구매 진행중</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>needle 선정 및 구매</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>기구물</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>악어클립은 사용하지 않음
-전용 GND 판 제작 예정</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>GND 판과의 연결 방법 협의 - 일단 악어클립으로 제작
-  - 악어클립 or Ring 단자</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>GND 판과의 연결 방법 협의</t>
+    <t>Reset IC 추가 - Voltage drop에 의한 MCU halt 방지</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -973,48 +973,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -1034,6 +992,48 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1414,7 +1414,7 @@
         <v>43188</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>33</v>
@@ -1423,10 +1423,10 @@
         <v>29</v>
       </c>
       <c r="G6" s="34" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
@@ -1435,7 +1435,7 @@
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>33</v>
@@ -1444,7 +1444,7 @@
         <v>29</v>
       </c>
       <c r="G7" s="34" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H7" s="14"/>
     </row>
@@ -1454,7 +1454,7 @@
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>33</v>
@@ -1463,10 +1463,10 @@
         <v>29</v>
       </c>
       <c r="G8" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
@@ -1475,7 +1475,7 @@
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>33</v>
@@ -1484,7 +1484,7 @@
         <v>29</v>
       </c>
       <c r="G9" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H9" s="14"/>
     </row>
@@ -1494,7 +1494,7 @@
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>33</v>
@@ -1503,7 +1503,7 @@
         <v>29</v>
       </c>
       <c r="G10" s="34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H10" s="14"/>
     </row>
@@ -1513,7 +1513,7 @@
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>33</v>
@@ -1522,7 +1522,7 @@
         <v>29</v>
       </c>
       <c r="G11" s="34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H11" s="14"/>
     </row>
@@ -1532,7 +1532,7 @@
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="49" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E12" s="50" t="s">
         <v>33</v>
@@ -1541,10 +1541,10 @@
         <v>29</v>
       </c>
       <c r="G12" s="51" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H12" s="52" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
@@ -1553,7 +1553,7 @@
       </c>
       <c r="C13" s="13"/>
       <c r="D13" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>33</v>
@@ -1562,7 +1562,7 @@
         <v>29</v>
       </c>
       <c r="G13" s="34" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H13" s="14"/>
     </row>
@@ -1572,7 +1572,7 @@
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>33</v>
@@ -1581,10 +1581,10 @@
         <v>29</v>
       </c>
       <c r="G14" s="34" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
@@ -1593,19 +1593,19 @@
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F15" s="39" t="s">
         <v>29</v>
       </c>
       <c r="G15" s="34" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
@@ -1782,8 +1782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H41"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1829,10 +1829,10 @@
       </c>
     </row>
     <row r="4" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B4" s="58">
+      <c r="B4" s="72">
         <v>1</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="69" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="48" t="s">
@@ -1842,18 +1842,18 @@
         <v>43153</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G4" s="28" t="s">
         <v>8</v>
       </c>
       <c r="H4" s="29" t="s">
-        <v>62</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B5" s="59"/>
-      <c r="C5" s="56"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="70"/>
       <c r="D5" s="44" t="s">
         <v>15</v>
       </c>
@@ -1864,13 +1864,13 @@
         <v>5</v>
       </c>
       <c r="G5" s="43" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H5" s="47"/>
     </row>
     <row r="6" spans="2:8" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="B6" s="59"/>
-      <c r="C6" s="56"/>
+      <c r="B6" s="73"/>
+      <c r="C6" s="70"/>
       <c r="D6" s="45" t="s">
         <v>14</v>
       </c>
@@ -1878,18 +1878,18 @@
         <v>43154</v>
       </c>
       <c r="F6" s="31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G6" s="32" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H6" s="33" t="s">
-        <v>64</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B7" s="60"/>
-      <c r="C7" s="57"/>
+      <c r="B7" s="74"/>
+      <c r="C7" s="71"/>
       <c r="D7" s="45" t="s">
         <v>14</v>
       </c>
@@ -1897,20 +1897,20 @@
         <v>43169</v>
       </c>
       <c r="F7" s="31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G7" s="37" t="s">
         <v>24</v>
       </c>
       <c r="H7" s="33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B8" s="66">
+      <c r="B8" s="80">
         <v>2</v>
       </c>
-      <c r="C8" s="65" t="s">
+      <c r="C8" s="79" t="s">
         <v>25</v>
       </c>
       <c r="D8" s="45" t="s">
@@ -1926,12 +1926,12 @@
         <v>12</v>
       </c>
       <c r="H8" s="41" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B9" s="59"/>
-      <c r="C9" s="56"/>
+      <c r="B9" s="73"/>
+      <c r="C9" s="70"/>
       <c r="D9" s="45" t="s">
         <v>15</v>
       </c>
@@ -1939,18 +1939,18 @@
         <v>43154</v>
       </c>
       <c r="F9" s="31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G9" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="H9" s="41" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="10" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B10" s="59"/>
-      <c r="C10" s="56"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="70"/>
       <c r="D10" s="45" t="s">
         <v>15</v>
       </c>
@@ -1958,18 +1958,18 @@
         <v>43188</v>
       </c>
       <c r="F10" s="31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G10" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="H10" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="H10" s="41" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="60"/>
-      <c r="C11" s="57"/>
+      <c r="B11" s="74"/>
+      <c r="C11" s="71"/>
       <c r="D11" s="44" t="s">
         <v>15</v>
       </c>
@@ -1980,18 +1980,18 @@
         <v>5</v>
       </c>
       <c r="G11" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="H11" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="20" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B12" s="63">
+      <c r="B12" s="77">
         <v>3</v>
       </c>
-      <c r="C12" s="61" t="s">
-        <v>48</v>
+      <c r="C12" s="75" t="s">
+        <v>47</v>
       </c>
       <c r="D12" s="45" t="s">
         <v>15</v>
@@ -2000,18 +2000,18 @@
         <v>43172</v>
       </c>
       <c r="F12" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="G12" s="37" t="s">
+      <c r="H12" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="H12" s="42" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="64"/>
-      <c r="C13" s="62"/>
+      <c r="B13" s="78"/>
+      <c r="C13" s="76"/>
       <c r="D13" s="44" t="s">
         <v>15</v>
       </c>
@@ -2020,16 +2020,16 @@
         <v>5</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H13" s="15"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="66">
+      <c r="B14" s="80">
         <v>4</v>
       </c>
-      <c r="C14" s="65" t="s">
-        <v>49</v>
+      <c r="C14" s="79" t="s">
+        <v>48</v>
       </c>
       <c r="D14" s="45" t="s">
         <v>15</v>
@@ -2038,18 +2038,18 @@
         <v>43158</v>
       </c>
       <c r="F14" s="31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G14" s="32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H14" s="42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B15" s="59"/>
-      <c r="C15" s="56"/>
+      <c r="B15" s="73"/>
+      <c r="C15" s="70"/>
       <c r="D15" s="45" t="s">
         <v>15</v>
       </c>
@@ -2060,15 +2060,15 @@
         <v>22</v>
       </c>
       <c r="G15" s="32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H15" s="38" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B16" s="59"/>
-      <c r="C16" s="56"/>
+      <c r="B16" s="73"/>
+      <c r="C16" s="70"/>
       <c r="D16" s="44" t="s">
         <v>15</v>
       </c>
@@ -2079,15 +2079,15 @@
         <v>5</v>
       </c>
       <c r="G16" s="19" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="H16" s="20" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="59"/>
-      <c r="C17" s="56"/>
+      <c r="B17" s="73"/>
+      <c r="C17" s="70"/>
       <c r="D17" s="45" t="s">
         <v>15</v>
       </c>
@@ -2098,16 +2098,16 @@
         <v>22</v>
       </c>
       <c r="G17" s="32" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H17" s="38"/>
     </row>
     <row r="18" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B18" s="54">
+      <c r="B18" s="68">
         <v>5</v>
       </c>
-      <c r="C18" s="53" t="s">
-        <v>52</v>
+      <c r="C18" s="67" t="s">
+        <v>51</v>
       </c>
       <c r="D18" s="46" t="s">
         <v>16</v>
@@ -2126,8 +2126,8 @@
       </c>
     </row>
     <row r="19" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B19" s="54"/>
-      <c r="C19" s="53"/>
+      <c r="B19" s="68"/>
+      <c r="C19" s="67"/>
       <c r="D19" s="46" t="s">
         <v>20</v>
       </c>
@@ -2145,8 +2145,8 @@
       </c>
     </row>
     <row r="20" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B20" s="54"/>
-      <c r="C20" s="53"/>
+      <c r="B20" s="68"/>
+      <c r="C20" s="67"/>
       <c r="D20" s="46" t="s">
         <v>17</v>
       </c>
@@ -2164,8 +2164,8 @@
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="54"/>
-      <c r="C21" s="53"/>
+      <c r="B21" s="68"/>
+      <c r="C21" s="67"/>
       <c r="D21" s="46" t="s">
         <v>26</v>
       </c>
@@ -2179,12 +2179,12 @@
         <v>27</v>
       </c>
       <c r="H21" s="42" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="54"/>
-      <c r="C22" s="53"/>
+      <c r="B22" s="68"/>
+      <c r="C22" s="67"/>
       <c r="D22" s="45" t="s">
         <v>26</v>
       </c>
@@ -2198,12 +2198,12 @@
         <v>12</v>
       </c>
       <c r="H22" s="42" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="54"/>
-      <c r="C23" s="53"/>
+      <c r="B23" s="68"/>
+      <c r="C23" s="67"/>
       <c r="D23" s="5"/>
       <c r="E23" s="13"/>
       <c r="F23" s="5"/>
@@ -2211,11 +2211,11 @@
       <c r="H23" s="15"/>
     </row>
     <row r="24" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B24" s="54">
+      <c r="B24" s="68">
         <v>6</v>
       </c>
-      <c r="C24" s="53" t="s">
-        <v>91</v>
+      <c r="C24" s="67" t="s">
+        <v>88</v>
       </c>
       <c r="D24" s="45" t="s">
         <v>15</v>
@@ -2224,18 +2224,18 @@
         <v>43171</v>
       </c>
       <c r="F24" s="31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G24" s="32" t="s">
         <v>34</v>
       </c>
       <c r="H24" s="38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="2:8" ht="33" x14ac:dyDescent="0.3">
-      <c r="B25" s="54"/>
-      <c r="C25" s="53"/>
+      <c r="B25" s="68"/>
+      <c r="C25" s="67"/>
       <c r="D25" s="44" t="s">
         <v>15</v>
       </c>
@@ -2243,16 +2243,16 @@
         <v>43175</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G25" s="19" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H25" s="15"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="54"/>
-      <c r="C26" s="53"/>
+      <c r="B26" s="68"/>
+      <c r="C26" s="67"/>
       <c r="D26" s="44" t="s">
         <v>15</v>
       </c>
@@ -2260,16 +2260,16 @@
         <v>43193</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G26" s="19" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H26" s="15"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="54"/>
-      <c r="C27" s="53"/>
+      <c r="B27" s="68"/>
+      <c r="C27" s="67"/>
       <c r="D27" s="44" t="s">
         <v>15</v>
       </c>
@@ -2277,16 +2277,16 @@
         <v>43193</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G27" s="19" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H27" s="15"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="54"/>
-      <c r="C28" s="53"/>
+      <c r="B28" s="68"/>
+      <c r="C28" s="67"/>
       <c r="D28" s="44"/>
       <c r="E28" s="13"/>
       <c r="F28" s="5"/>
@@ -2298,7 +2298,7 @@
         <v>7</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="13">
@@ -2308,7 +2308,7 @@
         <v>5</v>
       </c>
       <c r="G29" s="14" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H29" s="15"/>
     </row>
@@ -2458,7 +2458,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
@@ -2488,7 +2488,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>2</v>
@@ -2501,354 +2501,354 @@
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="67">
+      <c r="B6" s="53">
         <v>1</v>
       </c>
-      <c r="C6" s="78" t="s">
+      <c r="C6" s="64" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="64" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" s="61">
+        <v>43193</v>
+      </c>
+      <c r="F6" s="61">
+        <v>43206</v>
+      </c>
+      <c r="G6" s="64" t="s">
+        <v>80</v>
+      </c>
+      <c r="H6" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="78" t="s">
-        <v>82</v>
-      </c>
-      <c r="E6" s="75">
+      <c r="I6" s="55"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B7" s="56">
+        <v>2</v>
+      </c>
+      <c r="C7" s="65" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="65" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="62">
         <v>43193</v>
       </c>
-      <c r="F6" s="75">
+      <c r="F7" s="62">
         <v>43206</v>
       </c>
-      <c r="G6" s="78" t="s">
+      <c r="G7" s="65" t="s">
+        <v>80</v>
+      </c>
+      <c r="H7" s="57" t="s">
         <v>83</v>
       </c>
-      <c r="H6" s="68" t="s">
+      <c r="I7" s="58"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B8" s="56">
+        <v>3</v>
+      </c>
+      <c r="C8" s="65" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="65" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" s="62">
+        <v>43193</v>
+      </c>
+      <c r="F8" s="62">
+        <v>43206</v>
+      </c>
+      <c r="G8" s="65" t="s">
+        <v>80</v>
+      </c>
+      <c r="H8" s="57" t="s">
         <v>84</v>
       </c>
-      <c r="I6" s="69"/>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="70">
-        <v>2</v>
-      </c>
-      <c r="C7" s="79" t="s">
-        <v>81</v>
-      </c>
-      <c r="D7" s="79" t="s">
-        <v>82</v>
-      </c>
-      <c r="E7" s="76">
+      <c r="I8" s="58"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B9" s="56">
+        <v>4</v>
+      </c>
+      <c r="C9" s="65" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="65" t="s">
+        <v>79</v>
+      </c>
+      <c r="E9" s="62">
         <v>43193</v>
       </c>
-      <c r="F7" s="76">
+      <c r="F9" s="62">
         <v>43206</v>
       </c>
-      <c r="G7" s="79" t="s">
-        <v>83</v>
-      </c>
-      <c r="H7" s="71" t="s">
-        <v>86</v>
-      </c>
-      <c r="I7" s="72"/>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="70">
-        <v>3</v>
-      </c>
-      <c r="C8" s="79" t="s">
-        <v>81</v>
-      </c>
-      <c r="D8" s="79" t="s">
-        <v>82</v>
-      </c>
-      <c r="E8" s="76">
-        <v>43193</v>
-      </c>
-      <c r="F8" s="76">
-        <v>43206</v>
-      </c>
-      <c r="G8" s="79" t="s">
-        <v>83</v>
-      </c>
-      <c r="H8" s="71" t="s">
-        <v>87</v>
-      </c>
-      <c r="I8" s="72"/>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B9" s="70">
-        <v>4</v>
-      </c>
-      <c r="C9" s="79" t="s">
-        <v>81</v>
-      </c>
-      <c r="D9" s="79" t="s">
-        <v>82</v>
-      </c>
-      <c r="E9" s="76">
-        <v>43193</v>
-      </c>
-      <c r="F9" s="76">
-        <v>43206</v>
-      </c>
-      <c r="G9" s="79" t="s">
-        <v>83</v>
-      </c>
-      <c r="H9" s="71" t="s">
-        <v>88</v>
-      </c>
-      <c r="I9" s="72"/>
+      <c r="G9" s="65" t="s">
+        <v>80</v>
+      </c>
+      <c r="H9" s="57" t="s">
+        <v>85</v>
+      </c>
+      <c r="I9" s="58"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B10" s="70">
+      <c r="B10" s="56">
         <v>5</v>
       </c>
-      <c r="C10" s="79"/>
-      <c r="D10" s="79"/>
-      <c r="E10" s="76"/>
-      <c r="F10" s="76"/>
-      <c r="G10" s="79"/>
-      <c r="H10" s="71" t="s">
-        <v>94</v>
-      </c>
-      <c r="I10" s="72"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="65"/>
+      <c r="H10" s="57" t="s">
+        <v>91</v>
+      </c>
+      <c r="I10" s="58"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="70">
+      <c r="B11" s="56">
         <v>6</v>
       </c>
-      <c r="C11" s="79"/>
-      <c r="D11" s="79"/>
-      <c r="E11" s="76"/>
-      <c r="F11" s="76"/>
-      <c r="G11" s="79"/>
-      <c r="H11" s="71"/>
-      <c r="I11" s="72"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="65"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="58"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="70">
+      <c r="B12" s="56">
         <v>7</v>
       </c>
-      <c r="C12" s="79"/>
-      <c r="D12" s="79"/>
-      <c r="E12" s="76"/>
-      <c r="F12" s="76"/>
-      <c r="G12" s="79"/>
-      <c r="H12" s="71"/>
-      <c r="I12" s="72"/>
+      <c r="C12" s="65"/>
+      <c r="D12" s="65"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="62"/>
+      <c r="G12" s="65"/>
+      <c r="H12" s="57"/>
+      <c r="I12" s="58"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B13" s="70">
+      <c r="B13" s="56">
         <v>8</v>
       </c>
-      <c r="C13" s="79"/>
-      <c r="D13" s="79"/>
-      <c r="E13" s="76"/>
-      <c r="F13" s="76"/>
-      <c r="G13" s="79"/>
-      <c r="H13" s="71"/>
-      <c r="I13" s="72"/>
+      <c r="C13" s="65"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="65"/>
+      <c r="H13" s="57"/>
+      <c r="I13" s="58"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B14" s="70">
+      <c r="B14" s="56">
         <v>9</v>
       </c>
-      <c r="C14" s="79"/>
-      <c r="D14" s="79"/>
-      <c r="E14" s="76"/>
-      <c r="F14" s="76"/>
-      <c r="G14" s="79"/>
-      <c r="H14" s="71"/>
-      <c r="I14" s="72"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="62"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="57"/>
+      <c r="I14" s="58"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B15" s="70">
+      <c r="B15" s="56">
         <v>10</v>
       </c>
-      <c r="C15" s="79"/>
-      <c r="D15" s="79"/>
-      <c r="E15" s="76"/>
-      <c r="F15" s="76"/>
-      <c r="G15" s="79"/>
-      <c r="H15" s="71"/>
-      <c r="I15" s="72"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="62"/>
+      <c r="F15" s="62"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="57"/>
+      <c r="I15" s="58"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B16" s="70">
+      <c r="B16" s="56">
         <v>11</v>
       </c>
-      <c r="C16" s="79"/>
-      <c r="D16" s="79"/>
-      <c r="E16" s="76"/>
-      <c r="F16" s="76"/>
-      <c r="G16" s="79"/>
-      <c r="H16" s="71"/>
-      <c r="I16" s="72"/>
+      <c r="C16" s="65"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="62"/>
+      <c r="F16" s="62"/>
+      <c r="G16" s="65"/>
+      <c r="H16" s="57"/>
+      <c r="I16" s="58"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B17" s="70">
+      <c r="B17" s="56">
         <v>12</v>
       </c>
-      <c r="C17" s="79"/>
-      <c r="D17" s="79"/>
-      <c r="E17" s="76"/>
-      <c r="F17" s="76"/>
-      <c r="G17" s="79"/>
-      <c r="H17" s="71"/>
-      <c r="I17" s="72"/>
+      <c r="C17" s="65"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="62"/>
+      <c r="F17" s="62"/>
+      <c r="G17" s="65"/>
+      <c r="H17" s="57"/>
+      <c r="I17" s="58"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B18" s="70">
+      <c r="B18" s="56">
         <v>13</v>
       </c>
-      <c r="C18" s="79"/>
-      <c r="D18" s="79"/>
-      <c r="E18" s="76"/>
-      <c r="F18" s="76"/>
-      <c r="G18" s="79"/>
-      <c r="H18" s="71"/>
-      <c r="I18" s="72"/>
+      <c r="C18" s="65"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="62"/>
+      <c r="F18" s="62"/>
+      <c r="G18" s="65"/>
+      <c r="H18" s="57"/>
+      <c r="I18" s="58"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B19" s="70">
+      <c r="B19" s="56">
         <v>14</v>
       </c>
-      <c r="C19" s="79"/>
-      <c r="D19" s="79"/>
-      <c r="E19" s="76"/>
-      <c r="F19" s="76"/>
-      <c r="G19" s="79"/>
-      <c r="H19" s="71"/>
-      <c r="I19" s="72"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="65"/>
+      <c r="H19" s="57"/>
+      <c r="I19" s="58"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="70">
+      <c r="B20" s="56">
         <v>15</v>
       </c>
-      <c r="C20" s="79"/>
-      <c r="D20" s="79"/>
-      <c r="E20" s="76"/>
-      <c r="F20" s="76"/>
-      <c r="G20" s="79"/>
-      <c r="H20" s="71"/>
-      <c r="I20" s="72"/>
+      <c r="C20" s="65"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="62"/>
+      <c r="G20" s="65"/>
+      <c r="H20" s="57"/>
+      <c r="I20" s="58"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B21" s="70">
+      <c r="B21" s="56">
         <v>16</v>
       </c>
-      <c r="C21" s="79"/>
-      <c r="D21" s="79"/>
-      <c r="E21" s="76"/>
-      <c r="F21" s="76"/>
-      <c r="G21" s="79"/>
-      <c r="H21" s="71"/>
-      <c r="I21" s="72"/>
+      <c r="C21" s="65"/>
+      <c r="D21" s="65"/>
+      <c r="E21" s="62"/>
+      <c r="F21" s="62"/>
+      <c r="G21" s="65"/>
+      <c r="H21" s="57"/>
+      <c r="I21" s="58"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B22" s="70">
+      <c r="B22" s="56">
         <v>17</v>
       </c>
-      <c r="C22" s="79"/>
-      <c r="D22" s="79"/>
-      <c r="E22" s="76"/>
-      <c r="F22" s="76"/>
-      <c r="G22" s="79"/>
-      <c r="H22" s="71"/>
-      <c r="I22" s="72"/>
+      <c r="C22" s="65"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="62"/>
+      <c r="G22" s="65"/>
+      <c r="H22" s="57"/>
+      <c r="I22" s="58"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B23" s="70">
+      <c r="B23" s="56">
         <v>18</v>
       </c>
-      <c r="C23" s="79"/>
-      <c r="D23" s="79"/>
-      <c r="E23" s="76"/>
-      <c r="F23" s="76"/>
-      <c r="G23" s="79"/>
-      <c r="H23" s="71"/>
-      <c r="I23" s="72"/>
+      <c r="C23" s="65"/>
+      <c r="D23" s="65"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="62"/>
+      <c r="G23" s="65"/>
+      <c r="H23" s="57"/>
+      <c r="I23" s="58"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B24" s="70">
+      <c r="B24" s="56">
         <v>19</v>
       </c>
-      <c r="C24" s="79"/>
-      <c r="D24" s="79"/>
-      <c r="E24" s="76"/>
-      <c r="F24" s="76"/>
-      <c r="G24" s="79"/>
-      <c r="H24" s="71"/>
-      <c r="I24" s="72"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="62"/>
+      <c r="F24" s="62"/>
+      <c r="G24" s="65"/>
+      <c r="H24" s="57"/>
+      <c r="I24" s="58"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B25" s="70">
+      <c r="B25" s="56">
         <v>20</v>
       </c>
-      <c r="C25" s="79"/>
-      <c r="D25" s="79"/>
-      <c r="E25" s="76"/>
-      <c r="F25" s="76"/>
-      <c r="G25" s="79"/>
-      <c r="H25" s="71"/>
-      <c r="I25" s="72"/>
+      <c r="C25" s="65"/>
+      <c r="D25" s="65"/>
+      <c r="E25" s="62"/>
+      <c r="F25" s="62"/>
+      <c r="G25" s="65"/>
+      <c r="H25" s="57"/>
+      <c r="I25" s="58"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B26" s="70">
+      <c r="B26" s="56">
         <v>21</v>
       </c>
-      <c r="C26" s="79"/>
-      <c r="D26" s="79"/>
-      <c r="E26" s="76"/>
-      <c r="F26" s="76"/>
-      <c r="G26" s="79"/>
-      <c r="H26" s="71"/>
-      <c r="I26" s="72"/>
+      <c r="C26" s="65"/>
+      <c r="D26" s="65"/>
+      <c r="E26" s="62"/>
+      <c r="F26" s="62"/>
+      <c r="G26" s="65"/>
+      <c r="H26" s="57"/>
+      <c r="I26" s="58"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B27" s="70">
+      <c r="B27" s="56">
         <v>22</v>
       </c>
-      <c r="C27" s="79"/>
-      <c r="D27" s="79"/>
-      <c r="E27" s="76"/>
-      <c r="F27" s="76"/>
-      <c r="G27" s="79"/>
-      <c r="H27" s="71"/>
-      <c r="I27" s="72"/>
+      <c r="C27" s="65"/>
+      <c r="D27" s="65"/>
+      <c r="E27" s="62"/>
+      <c r="F27" s="62"/>
+      <c r="G27" s="65"/>
+      <c r="H27" s="57"/>
+      <c r="I27" s="58"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B28" s="70">
+      <c r="B28" s="56">
         <v>23</v>
       </c>
-      <c r="C28" s="79"/>
-      <c r="D28" s="79"/>
-      <c r="E28" s="76"/>
-      <c r="F28" s="76"/>
-      <c r="G28" s="79"/>
-      <c r="H28" s="71"/>
-      <c r="I28" s="72"/>
+      <c r="C28" s="65"/>
+      <c r="D28" s="65"/>
+      <c r="E28" s="62"/>
+      <c r="F28" s="62"/>
+      <c r="G28" s="65"/>
+      <c r="H28" s="57"/>
+      <c r="I28" s="58"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B29" s="70">
+      <c r="B29" s="56">
         <v>24</v>
       </c>
-      <c r="C29" s="79"/>
-      <c r="D29" s="79"/>
-      <c r="E29" s="76"/>
-      <c r="F29" s="76"/>
-      <c r="G29" s="79"/>
-      <c r="H29" s="71"/>
-      <c r="I29" s="72"/>
+      <c r="C29" s="65"/>
+      <c r="D29" s="65"/>
+      <c r="E29" s="62"/>
+      <c r="F29" s="62"/>
+      <c r="G29" s="65"/>
+      <c r="H29" s="57"/>
+      <c r="I29" s="58"/>
     </row>
     <row r="30" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="70">
+      <c r="B30" s="56">
         <v>25</v>
       </c>
-      <c r="C30" s="80"/>
-      <c r="D30" s="80"/>
-      <c r="E30" s="77"/>
-      <c r="F30" s="77"/>
-      <c r="G30" s="80"/>
-      <c r="H30" s="73"/>
-      <c r="I30" s="74"/>
+      <c r="C30" s="66"/>
+      <c r="D30" s="66"/>
+      <c r="E30" s="63"/>
+      <c r="F30" s="63"/>
+      <c r="G30" s="66"/>
+      <c r="H30" s="59"/>
+      <c r="I30" s="60"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>